<commit_message>
[ADD] model_ng & Experimental_data_ds.xlsx
</commit_message>
<xml_diff>
--- a/data/experimental/Experimental_data_ds.xlsx
+++ b/data/experimental/Experimental_data_ds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bisbii\PythonProjects\model_analysis\data\experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8436AE4-193B-4248-9962-0CD3CC8C1EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7EE40E-2BB4-4A1E-A2D9-572ED2D75740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Km</t>
   </si>
@@ -60,6 +60,45 @@
   </si>
   <si>
     <t>g/cell</t>
+  </si>
+  <si>
+    <t>initial ext</t>
+  </si>
+  <si>
+    <t>initial int</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>mmol/l</t>
+  </si>
+  <si>
+    <t>mmol/gDW</t>
+  </si>
+  <si>
+    <t>final ext</t>
+  </si>
+  <si>
+    <t>final_biomass</t>
+  </si>
+  <si>
+    <t>comp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> g/L</t>
+  </si>
+  <si>
+    <t>nitrate in biomass</t>
+  </si>
+  <si>
+    <t>mmol/L</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0960852414012486#ab005</t>
   </si>
 </sst>
 </file>
@@ -377,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:M22"/>
+  <dimension ref="A3:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +427,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -399,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -414,7 +453,7 @@
         <v>2.0967741935483869E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -430,8 +469,17 @@
         <f>0.057/14*1000</f>
         <v>4.0714285714285712</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S6">
+        <f>11.95*0.25+18*0.1+11.05*0.45+8*0.2</f>
+        <v>11.36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -446,7 +494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -457,7 +505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -470,8 +518,8 @@
         <v>1.4E-3</v>
       </c>
       <c r="D11">
-        <f>AVERAGE(B11:C11)</f>
-        <v>1.25E-3</v>
+        <f>AVERAGE(B11:C11,E11:F11)</f>
+        <v>2.0374999999999998E-3</v>
       </c>
       <c r="E11">
         <f>1.85/1000</f>
@@ -482,7 +530,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -499,34 +547,134 @@
         <v>9.411764705882355</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K14">
         <f>0.03/14*1000</f>
         <v>2.1428571428571428</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K15">
         <f>0.07/14*1000</f>
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K17">
         <f>0.021/14*1000</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K18">
         <f>0.101/14*1000</f>
         <v>7.2142857142857144</v>
       </c>
-    </row>
-    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <v>0.11799999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19">
+        <v>10</v>
+      </c>
+      <c r="R19" t="s">
+        <v>11</v>
+      </c>
+      <c r="T19">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="20" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K22">
         <f>0.19*24</f>
         <v>4.5600000000000005</v>
+      </c>
+      <c r="P22" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q22">
+        <f>10-7.5</f>
+        <v>2.5</v>
+      </c>
+      <c r="R22" t="s">
+        <v>11</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q24">
+        <v>1.024</v>
+      </c>
+      <c r="R24" t="s">
+        <v>16</v>
+      </c>
+      <c r="T24">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="25" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q25">
+        <v>4.42</v>
+      </c>
+      <c r="R25" t="s">
+        <v>12</v>
+      </c>
+      <c r="T25">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="27" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q27">
+        <f>Q24*Q25</f>
+        <v>4.5260800000000003</v>
+      </c>
+      <c r="R27" t="s">
+        <v>18</v>
+      </c>
+      <c r="T27">
+        <f>T25*T24</f>
+        <v>7.7792000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="T29">
+        <f>T27-T19</f>
+        <v>0.27920000000000034</v>
+      </c>
+    </row>
+    <row r="30" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <f>T29/T18</f>
+        <v>2.3661016949152573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] refactor & merge with main
</commit_message>
<xml_diff>
--- a/data/experimental/Experimental_data_ds.xlsx
+++ b/data/experimental/Experimental_data_ds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bisbii\PythonProjects\model_analysis\data\experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7EE40E-2BB4-4A1E-A2D9-572ED2D75740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0D7201-EFBB-413E-BB29-E66640698519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A3:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>